<commit_message>
Added the sprint backlog
</commit_message>
<xml_diff>
--- a/sprints/sprint1/Sprint 1 Backlog Burndown.xlsx
+++ b/sprints/sprint1/Sprint 1 Backlog Burndown.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
   <si>
     <t>Related User Story</t>
   </si>
@@ -92,6 +92,12 @@
   </si>
   <si>
     <t>Develop functionality that allows HR to view a master list of all employees</t>
+  </si>
+  <si>
+    <t>User wants to view landing page</t>
+  </si>
+  <si>
+    <t>Create UI for landing page</t>
   </si>
   <si>
     <t>Estimate Totals</t>
@@ -248,25 +254,29 @@
     <xf borderId="8" fillId="4" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="8" fillId="4" fontId="0" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="8" fillId="5" fontId="0" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
+    <xf borderId="8" fillId="5" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="2" fillId="4" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="2" fillId="4" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="4" fontId="0" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="5" fontId="0" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="2" fillId="5" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
+    <xf borderId="2" fillId="4" fontId="0" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="2" fillId="4" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
+    <xf borderId="2" fillId="5" fontId="0" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="2" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="right" shrinkToFit="0" wrapText="1"/>
     </xf>
@@ -338,11 +348,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1189754571"/>
-        <c:axId val="1028965459"/>
+        <c:axId val="1579986528"/>
+        <c:axId val="1694766446"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1189754571"/>
+        <c:axId val="1579986528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -394,10 +404,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1028965459"/>
+        <c:crossAx val="1694766446"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1028965459"/>
+        <c:axId val="1694766446"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -461,7 +471,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1189754571"/>
+        <c:crossAx val="1579986528"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
@@ -767,302 +777,388 @@
       <c r="C4" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="14"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
+      <c r="D4" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="E4" s="14">
+        <v>1.0</v>
+      </c>
+      <c r="F4" s="14">
+        <v>0.0</v>
+      </c>
+      <c r="G4" s="14">
+        <v>0.0</v>
+      </c>
+      <c r="H4" s="14">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="18"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
+      <c r="D5" s="15">
+        <v>10.0</v>
+      </c>
+      <c r="E5" s="17">
+        <v>10.0</v>
+      </c>
+      <c r="F5" s="17">
+        <v>4.0</v>
+      </c>
+      <c r="G5" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="H5" s="17">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="18"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
+      <c r="D6" s="15">
+        <v>7.0</v>
+      </c>
+      <c r="E6" s="17">
+        <v>7.0</v>
+      </c>
+      <c r="F6" s="17">
+        <v>3.0</v>
+      </c>
+      <c r="G6" s="17">
+        <v>3.0</v>
+      </c>
+      <c r="H6" s="17">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="18"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
+      <c r="D7" s="15">
+        <v>2.0</v>
+      </c>
+      <c r="E7" s="17">
+        <v>2.0</v>
+      </c>
+      <c r="F7" s="17">
+        <v>1.0</v>
+      </c>
+      <c r="G7" s="17">
+        <v>1.0</v>
+      </c>
+      <c r="H7" s="17">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
+      <c r="D8" s="15">
+        <v>5.0</v>
+      </c>
+      <c r="E8" s="17">
+        <v>5.0</v>
+      </c>
+      <c r="F8" s="17">
+        <v>2.0</v>
+      </c>
+      <c r="G8" s="17">
+        <v>1.0</v>
+      </c>
+      <c r="H8" s="17">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
+      <c r="D9" s="15">
+        <v>4.0</v>
+      </c>
+      <c r="E9" s="17">
+        <v>4.0</v>
+      </c>
+      <c r="F9" s="17">
+        <v>4.0</v>
+      </c>
+      <c r="G9" s="17">
+        <v>2.0</v>
+      </c>
+      <c r="H9" s="17">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
+      <c r="D10" s="15">
+        <v>8.0</v>
+      </c>
+      <c r="E10" s="17">
+        <v>7.0</v>
+      </c>
+      <c r="F10" s="17">
+        <v>6.0</v>
+      </c>
+      <c r="G10" s="17">
+        <v>4.0</v>
+      </c>
+      <c r="H10" s="17">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="11">
-      <c r="A11" s="18"/>
-      <c r="B11" s="22"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
+      <c r="A11" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="15">
+        <v>3.0</v>
+      </c>
+      <c r="E11" s="17">
+        <v>3.0</v>
+      </c>
+      <c r="F11" s="17">
+        <v>3.0</v>
+      </c>
+      <c r="G11" s="17">
+        <v>0.0</v>
+      </c>
+      <c r="H11" s="17">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="12">
-      <c r="A12" s="18"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
+      <c r="A12" s="20"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
     </row>
     <row r="13">
-      <c r="A13" s="18"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
+      <c r="A13" s="20"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="22"/>
     </row>
     <row r="14">
-      <c r="A14" s="18"/>
-      <c r="B14" s="22"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
+      <c r="A14" s="20"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
     </row>
     <row r="15">
-      <c r="A15" s="18"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19"/>
+      <c r="A15" s="20"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
     </row>
     <row r="16">
-      <c r="A16" s="18"/>
-      <c r="B16" s="22"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
+      <c r="A16" s="20"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
     </row>
     <row r="17">
-      <c r="A17" s="18"/>
-      <c r="B17" s="22"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
+      <c r="A17" s="20"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
     </row>
     <row r="18">
-      <c r="A18" s="18"/>
-      <c r="B18" s="22"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
+      <c r="A18" s="20"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
     </row>
     <row r="19">
-      <c r="A19" s="18"/>
-      <c r="B19" s="22"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="19"/>
+      <c r="A19" s="20"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
     </row>
     <row r="20">
-      <c r="A20" s="18"/>
-      <c r="B20" s="22"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
+      <c r="A20" s="20"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="22"/>
     </row>
     <row r="21">
-      <c r="A21" s="18"/>
-      <c r="B21" s="22"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="19"/>
+      <c r="A21" s="20"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="22"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="18"/>
-      <c r="B22" s="22"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
+      <c r="A22" s="20"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="22"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="18"/>
-      <c r="B23" s="22"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
+      <c r="A23" s="20"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="18"/>
-      <c r="B24" s="22"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="19"/>
+      <c r="A24" s="20"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="22"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="18"/>
-      <c r="B25" s="22"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
+      <c r="A25" s="20"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="22"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="18"/>
-      <c r="B26" s="22"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="19"/>
+      <c r="A26" s="20"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="22"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="18"/>
-      <c r="B27" s="22"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="19"/>
-      <c r="G27" s="19"/>
-      <c r="H27" s="19"/>
+      <c r="A27" s="20"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="B28" s="23" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C28" s="24"/>
       <c r="D28" s="24">
         <f t="shared" ref="D28:H28" si="1">SUM(D4:D27)</f>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="E28" s="24">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="F28" s="24">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="G28" s="24">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="H28" s="24">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
@@ -3986,10 +4082,10 @@
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="E1:H1"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="B1:B3"/>
     <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:H1"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>